<commit_message>
Manejo de data aleatoria con excel
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/UserData.xlsx
+++ b/src/main/resources/Data/UserData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SQA\Desktop\Projects\Terminales\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED927459-8530-4621-8652-100DC94C58F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4712E89-CCB3-48F2-AFAC-9D2DA5A4C5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8916" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Nombre</t>
   </si>
@@ -45,15 +45,6 @@
     <t>Cedula</t>
   </si>
   <si>
-    <t>calle</t>
-  </si>
-  <si>
-    <t>numero</t>
-  </si>
-  <si>
-    <t>placa</t>
-  </si>
-  <si>
     <t>Barrio</t>
   </si>
   <si>
@@ -69,20 +60,89 @@
     <t>Numero Orden</t>
   </si>
   <si>
-    <t>Pruebas</t>
-  </si>
-  <si>
     <t>Excel@excel.com</t>
   </si>
   <si>
+    <t>Calle</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>Placa</t>
+  </si>
+  <si>
+    <t>Cod_Calle</t>
+  </si>
+  <si>
+    <t>1486464778355100116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barrio 20 de julio </t>
+  </si>
+  <si>
+    <t>Complemento</t>
+  </si>
+  <si>
+    <t>Casa 1</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
     <t>Juan</t>
+  </si>
+  <si>
+    <t>uno</t>
+  </si>
+  <si>
+    <t>dos</t>
+  </si>
+  <si>
+    <t>tres</t>
+  </si>
+  <si>
+    <t>cuatro</t>
+  </si>
+  <si>
+    <t>cinco</t>
+  </si>
+  <si>
+    <t>seis</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>114a</t>
+  </si>
+  <si>
+    <t>Suba</t>
+  </si>
+  <si>
+    <t>1486464778355100910</t>
+  </si>
+  <si>
+    <t>BQU K</t>
+  </si>
+  <si>
+    <t>OFI  1</t>
+  </si>
+  <si>
+    <t>Casa 2</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Detalle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,19 +158,65 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -120,9 +226,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -404,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,42 +544,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2">
         <v>888888881</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3001111111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2">
+        <v>888888882</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3002222222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2">
+        <v>888888883</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2">
         <v>30033333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2">
+        <v>888888884</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3004444444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2">
+        <v>888888885</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3005555555</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2">
+        <v>888888886</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3006666666</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{0E2BE8BC-56A9-4E8B-A804-F8C86B992813}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{6B12FFA7-5F28-4F77-8572-B29AD85D23E9}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{D9899037-80E8-4BA1-ADDF-DC3C86A75654}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{538808ED-1061-443C-A9D7-923F1E46795B}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{D871DFCA-D73E-4C8C-A64B-48B9A01FC725}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{EFFB3308-DF78-4A0B-8282-E3D820499048}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -461,44 +677,136 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451B7164-E691-4746-A6A7-6F76F30433F2}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="C1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C2">
+      <c r="E2" s="4">
+        <v>27</v>
+      </c>
+      <c r="F2" s="4">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E2">
-        <v>7</v>
-      </c>
+      <c r="D3" s="5">
+        <v>60</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="5">
+        <v>50</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -553,13 +861,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manejo de dirección con complementos
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/UserData.xlsx
+++ b/src/main/resources/Data/UserData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SQA\Desktop\Projects\Terminales\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4712E89-CCB3-48F2-AFAC-9D2DA5A4C5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B0F9EA-6F3B-45C3-8330-80F17913C31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>Nombre</t>
   </si>
@@ -126,9 +126,6 @@
     <t>BQU K</t>
   </si>
   <si>
-    <t>OFI  1</t>
-  </si>
-  <si>
     <t>Casa 2</t>
   </si>
   <si>
@@ -136,6 +133,30 @@
   </si>
   <si>
     <t>Detalle</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>Camping</t>
+  </si>
+  <si>
+    <t>OFI 1</t>
+  </si>
+  <si>
+    <t>115a</t>
+  </si>
+  <si>
+    <t>Casa 3</t>
+  </si>
+  <si>
+    <t>OFI 2</t>
   </si>
 </sst>
 </file>
@@ -532,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -677,10 +698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451B7164-E691-4746-A6A7-6F76F30433F2}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,10 +739,10 @@
         <v>17</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -755,53 +776,124 @@
         <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D4" s="5">
         <v>60</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="5">
-        <v>50</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="F4" s="5">
+        <v>55</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4">
+        <v>27</v>
+      </c>
+      <c r="F5" s="4">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5">
+        <v>61</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="5">
+        <v>56</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
flujo con producto random y datos random
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/UserData.xlsx
+++ b/src/main/resources/Data/UserData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SQA\Desktop\Projects\Terminales\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B0F9EA-6F3B-45C3-8330-80F17913C31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA07873-8574-4726-9DE4-35BCF2B4B2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,28 @@
     <sheet name="Epayco" sheetId="2" r:id="rId3"/>
     <sheet name="Equipo" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
   <si>
     <t>Nombre</t>
   </si>
@@ -157,6 +168,9 @@
   </si>
   <si>
     <t>OFI 2</t>
+  </si>
+  <si>
+    <t>Banco</t>
   </si>
 </sst>
 </file>
@@ -553,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,15 +918,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0468305-F41E-4C0A-A56F-424EEFB5CC16}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -928,8 +942,34 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2">
+        <v>888888881</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3001111111</v>
+      </c>
+      <c r="F2">
+        <v>1001</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{2F7D7575-B7D9-4905-A67D-A561DA5B1F26}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Flujo de marcas añadido
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/UserData.xlsx
+++ b/src/main/resources/Data/UserData.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SQA\Desktop\Projects\Terminales\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA07873-8574-4726-9DE4-35BCF2B4B2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9B8CD0-4358-42A7-BBF0-692858299C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
     <sheet name="Direccion" sheetId="3" r:id="rId2"/>
     <sheet name="Epayco" sheetId="2" r:id="rId3"/>
     <sheet name="Equipo" sheetId="4" r:id="rId4"/>
+    <sheet name="Ambiente" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>Nombre</t>
   </si>
@@ -171,6 +172,21 @@
   </si>
   <si>
     <t>Banco</t>
+  </si>
+  <si>
+    <t>URL Pruebas</t>
+  </si>
+  <si>
+    <t>URL Produccion</t>
+  </si>
+  <si>
+    <t>https://integration-5ojmyuq-jvrr247te2phq.us-5.magentosite.cloud/celulares.html</t>
+  </si>
+  <si>
+    <t>https://tienda.movistar.com.co/celulares.html</t>
+  </si>
+  <si>
+    <t>URL</t>
   </si>
 </sst>
 </file>
@@ -261,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -284,6 +300,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -918,9 +935,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0468305-F41E-4C0A-A56F-424EEFB5CC16}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -964,6 +981,11 @@
       </c>
       <c r="F2">
         <v>1001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>1077</v>
       </c>
     </row>
   </sheetData>
@@ -979,11 +1001,12 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
   </cols>
@@ -1005,4 +1028,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A1884-B518-4DD3-9D9A-D735AA23AF02}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="68.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{6BA2835B-1F97-461E-876C-CB56A4F3FF7A}">
+      <formula1>$A$2:$B$2</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{33169BB5-59F2-4050-AF08-9E070D4CCD5C}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{1D0A0871-8286-4693-9864-7A2BD29B4F49}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>